<commit_message>
reviewed RTP project list
</commit_message>
<xml_diff>
--- a/projlist/2040 Project List_Consolidated draft with AQ (ORIGINAL).xlsx
+++ b/projlist/2040 Project List_Consolidated draft with AQ (ORIGINAL).xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\GitHub\RTP\projlist\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02F2B836-E8C0-4D41-ADC2-B61A829DE709}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="285" windowWidth="19440" windowHeight="11640" tabRatio="742" firstSheet="5" activeTab="11"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" tabRatio="742" firstSheet="15" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Auto Constrained - Arterial Lin" sheetId="1" r:id="rId1"/>
@@ -298,22 +304,33 @@
     <definedName name="Z_E02D8BBA_373C_430A_B0C6_EFAFB65B79B1_.wvu.PrintTitles" localSheetId="12" hidden="1">'Transit Constrained'!$4:$4</definedName>
     <definedName name="Z_E02D8BBA_373C_430A_B0C6_EFAFB65B79B1_.wvu.PrintTitles" localSheetId="13" hidden="1">'Transit Illustrative'!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Lane County - Personal View" guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1280" windowHeight="705" tabRatio="742" activeSheetId="5"/>
+    <customWorkbookView name="CLARKE Kelly A - Personal View" guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" mergeInterval="0" personalView="1" xWindow="77" yWindow="23" windowWidth="1705" windowHeight="855" tabRatio="742" activeSheetId="1"/>
     <customWorkbookView name="THOMPSON Paul E - Personal View" guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1916" windowHeight="855" tabRatio="742" activeSheetId="1"/>
-    <customWorkbookView name="CLARKE Kelly A - Personal View" guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" mergeInterval="0" personalView="1" xWindow="77" yWindow="23" windowWidth="1705" windowHeight="855" tabRatio="742" activeSheetId="1"/>
-    <customWorkbookView name="Lane County - Personal View" guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1280" windowHeight="705" tabRatio="742" activeSheetId="5"/>
   </customWorkbookViews>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CLARKE Kelly A</author>
   </authors>
   <commentList>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -351,12 +368,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CLARKE Kelly A</author>
   </authors>
   <commentList>
-    <comment ref="C23" authorId="0">
+    <comment ref="C23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -386,12 +403,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CLARKE Kelly A</author>
   </authors>
   <commentList>
-    <comment ref="C31" authorId="0">
+    <comment ref="C31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -423,12 +440,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CLARKE Kelly A</author>
   </authors>
   <commentList>
-    <comment ref="L4" authorId="0">
+    <comment ref="L4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000001000000}">
       <text>
         <r>
           <rPr>
@@ -452,7 +469,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L15" authorId="0">
+    <comment ref="L15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000002000000}">
       <text>
         <r>
           <rPr>
@@ -476,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K46" authorId="0">
+    <comment ref="K46" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0400-000003000000}">
       <text>
         <r>
           <rPr>
@@ -505,12 +522,12 @@
 </file>
 
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CLARKE Kelly A</author>
   </authors>
   <commentList>
-    <comment ref="F4" authorId="0">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0F00-000001000000}">
       <text>
         <r>
           <rPr>
@@ -540,12 +557,12 @@
 </file>
 
 <file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CLARKE Kelly A</author>
   </authors>
   <commentList>
-    <comment ref="N14" authorId="0">
+    <comment ref="N14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-1600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -574,7 +591,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2989" uniqueCount="1244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2990" uniqueCount="1244">
   <si>
     <t>Name</t>
   </si>
@@ -4532,21 +4549,6 @@
     <t>PB6. Cost estimated using PB-18</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Estimated Cost (2016) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>$- cost indicates project cost is included in another project in the RTP</t>
-    </r>
-  </si>
-  <si>
     <t>* Italicized construction year windows need to be confirmed by Eugene</t>
   </si>
   <si>
@@ -4567,12 +4569,15 @@
   <si>
     <t>Springfield TSP 
 #US-15</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
     <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
@@ -4582,7 +4587,7 @@
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="51" x14ac:knownFonts="1">
+  <fonts count="50" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -4894,13 +4899,6 @@
     <font>
       <i/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -6657,6 +6655,21 @@
     <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6716,40 +6729,28 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Comma" xfId="8" builtinId="3"/>
-    <cellStyle name="Comma 2" xfId="9"/>
+    <cellStyle name="Comma 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
-    <cellStyle name="Currency 2" xfId="5"/>
+    <cellStyle name="Currency 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 2 2" xfId="3"/>
-    <cellStyle name="Normal 2 2 2" xfId="6"/>
-    <cellStyle name="Normal 3" xfId="4"/>
-    <cellStyle name="Normal 4" xfId="7"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normal 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -6798,7 +6799,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6831,9 +6832,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -6866,6 +6884,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7041,7 +7076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor indexed="15"/>
     <pageSetUpPr fitToPage="1"/>
@@ -7049,7 +7084,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7073,38 +7108,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="527" t="s">
+      <c r="A1" s="532" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="527"/>
-      <c r="C1" s="527"/>
-      <c r="D1" s="527"/>
-      <c r="E1" s="527"/>
-      <c r="F1" s="527"/>
-      <c r="G1" s="527"/>
-      <c r="H1" s="527"/>
-      <c r="I1" s="527"/>
-      <c r="J1" s="527"/>
-      <c r="K1" s="527"/>
-      <c r="L1" s="527"/>
+      <c r="B1" s="532"/>
+      <c r="C1" s="532"/>
+      <c r="D1" s="532"/>
+      <c r="E1" s="532"/>
+      <c r="F1" s="532"/>
+      <c r="G1" s="532"/>
+      <c r="H1" s="532"/>
+      <c r="I1" s="532"/>
+      <c r="J1" s="532"/>
+      <c r="K1" s="532"/>
+      <c r="L1" s="532"/>
       <c r="M1" s="89"/>
       <c r="N1" s="89"/>
     </row>
     <row r="2" spans="1:19" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="528" t="s">
+      <c r="A2" s="533" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="528"/>
-      <c r="C2" s="528"/>
-      <c r="D2" s="528"/>
-      <c r="E2" s="528"/>
-      <c r="F2" s="528"/>
-      <c r="G2" s="528"/>
-      <c r="H2" s="528"/>
-      <c r="I2" s="528"/>
-      <c r="J2" s="528"/>
-      <c r="K2" s="528"/>
-      <c r="L2" s="528"/>
+      <c r="B2" s="533"/>
+      <c r="C2" s="533"/>
+      <c r="D2" s="533"/>
+      <c r="E2" s="533"/>
+      <c r="F2" s="533"/>
+      <c r="G2" s="533"/>
+      <c r="H2" s="533"/>
+      <c r="I2" s="533"/>
+      <c r="J2" s="533"/>
+      <c r="K2" s="533"/>
+      <c r="L2" s="533"/>
     </row>
     <row r="3" spans="1:19" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
@@ -7145,10 +7180,10 @@
       <c r="H4" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="I4" s="529" t="s">
+      <c r="I4" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="J4" s="529"/>
+      <c r="J4" s="534"/>
       <c r="K4" s="61" t="s">
         <v>2</v>
       </c>
@@ -7169,13 +7204,13 @@
       </c>
     </row>
     <row r="5" spans="1:19" s="6" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="530" t="s">
+      <c r="A5" s="535" t="s">
         <v>309</v>
       </c>
-      <c r="B5" s="531"/>
-      <c r="C5" s="531"/>
-      <c r="D5" s="531"/>
-      <c r="E5" s="531"/>
+      <c r="B5" s="536"/>
+      <c r="C5" s="536"/>
+      <c r="D5" s="536"/>
+      <c r="E5" s="536"/>
       <c r="F5" s="494"/>
       <c r="G5" s="494"/>
       <c r="H5" s="494"/>
@@ -7399,28 +7434,28 @@
       <c r="D25" s="392"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:L7"/>
+  <autoFilter ref="A4:L7" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="71" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D4" sqref="D4"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="71" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="A5" sqref="A5:K5"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="81" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="49" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="75" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="A6" sqref="A6"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="49" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="71" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="A5" sqref="A5:K5"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="71" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D4" sqref="D4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="49" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="81" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="4">
@@ -7431,7 +7466,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H10 H24">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H10 H24" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -7444,7 +7479,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7496,10 +7531,10 @@
       <c r="H1" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="529" t="s">
+      <c r="I1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="529"/>
+      <c r="J1" s="534"/>
       <c r="K1" s="73" t="s">
         <v>2</v>
       </c>
@@ -7517,20 +7552,20 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="545" t="s">
         <v>312</v>
       </c>
-      <c r="B2" s="540"/>
-      <c r="C2" s="540"/>
-      <c r="D2" s="540"/>
-      <c r="E2" s="540"/>
-      <c r="F2" s="540"/>
-      <c r="G2" s="540"/>
-      <c r="H2" s="540"/>
-      <c r="I2" s="540"/>
-      <c r="J2" s="540"/>
-      <c r="K2" s="540"/>
-      <c r="L2" s="540"/>
+      <c r="B2" s="545"/>
+      <c r="C2" s="545"/>
+      <c r="D2" s="545"/>
+      <c r="E2" s="545"/>
+      <c r="F2" s="545"/>
+      <c r="G2" s="545"/>
+      <c r="H2" s="545"/>
+      <c r="I2" s="545"/>
+      <c r="J2" s="545"/>
+      <c r="K2" s="545"/>
+      <c r="L2" s="545"/>
     </row>
     <row r="3" spans="1:15" s="86" customFormat="1" ht="135" x14ac:dyDescent="0.2">
       <c r="A3" s="327" t="s">
@@ -7549,7 +7584,7 @@
         <v>1181</v>
       </c>
       <c r="F3" s="349"/>
-      <c r="G3" s="551">
+      <c r="G3" s="531">
         <v>685000000</v>
       </c>
       <c r="H3" s="350" t="s">
@@ -7575,8 +7610,8 @@
       <c r="N3" s="150" t="s">
         <v>1226</v>
       </c>
-      <c r="O3" s="549" t="s">
-        <v>1240</v>
+      <c r="O3" s="529" t="s">
+        <v>1239</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="86" customFormat="1" ht="75" x14ac:dyDescent="0.2">
@@ -7771,7 +7806,7 @@
     </row>
     <row r="8" spans="1:15" s="322" customFormat="1" ht="120" x14ac:dyDescent="0.2">
       <c r="A8" s="377" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="B8" s="377" t="s">
         <v>1110</v>
@@ -7788,7 +7823,7 @@
       <c r="F8" s="381" t="s">
         <v>1112</v>
       </c>
-      <c r="G8" s="548">
+      <c r="G8" s="528">
         <v>10000000</v>
       </c>
       <c r="H8" s="463" t="s">
@@ -7811,11 +7846,11 @@
       <c r="M8" s="451" t="s">
         <v>1186</v>
       </c>
-      <c r="N8" s="550" t="s">
-        <v>1243</v>
-      </c>
-      <c r="O8" s="549" t="s">
-        <v>1241</v>
+      <c r="N8" s="530" t="s">
+        <v>1242</v>
+      </c>
+      <c r="O8" s="529" t="s">
+        <v>1240</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="322" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -7858,28 +7893,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L10"/>
+  <autoFilter ref="A1:L10" xr:uid="{00000000-0009-0000-0000-000009000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="A4" sqref="A4:E4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="75" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="47" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="80" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="B4" sqref="B4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="47" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="A4" sqref="A4:E4"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="47" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="75" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -7888,7 +7923,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H8" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -7901,7 +7936,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -7953,10 +7988,10 @@
       <c r="H1" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="529" t="s">
+      <c r="I1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="529"/>
+      <c r="J1" s="534"/>
       <c r="K1" s="73" t="s">
         <v>2</v>
       </c>
@@ -7975,20 +8010,20 @@
       <c r="P1" s="89"/>
     </row>
     <row r="2" spans="1:16" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="545" t="s">
         <v>311</v>
       </c>
-      <c r="B2" s="540"/>
-      <c r="C2" s="540"/>
-      <c r="D2" s="540"/>
-      <c r="E2" s="540"/>
-      <c r="F2" s="540"/>
-      <c r="G2" s="540"/>
-      <c r="H2" s="540"/>
-      <c r="I2" s="540"/>
-      <c r="J2" s="540"/>
-      <c r="K2" s="540"/>
-      <c r="L2" s="540"/>
+      <c r="B2" s="545"/>
+      <c r="C2" s="545"/>
+      <c r="D2" s="545"/>
+      <c r="E2" s="545"/>
+      <c r="F2" s="545"/>
+      <c r="G2" s="545"/>
+      <c r="H2" s="545"/>
+      <c r="I2" s="545"/>
+      <c r="J2" s="545"/>
+      <c r="K2" s="545"/>
+      <c r="L2" s="545"/>
     </row>
     <row r="3" spans="1:16" s="85" customFormat="1" ht="135" x14ac:dyDescent="0.2">
       <c r="A3" s="137" t="s">
@@ -8217,7 +8252,7 @@
         <v>1109</v>
       </c>
     </row>
-    <row r="8" spans="1:16" s="85" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" s="85" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A8" s="137" t="s">
         <v>18</v>
       </c>
@@ -8330,28 +8365,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L9"/>
+  <autoFilter ref="A1:L9" xr:uid="{00000000-0009-0000-0000-00000A000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="75" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="46" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="80" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="46" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
       <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="46" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="75" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -8360,7 +8395,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H9" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -8373,14 +8408,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8426,10 +8461,10 @@
       <c r="H1" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="529" t="s">
+      <c r="I1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="529"/>
+      <c r="J1" s="534"/>
       <c r="K1" s="73" t="s">
         <v>2</v>
       </c>
@@ -8447,20 +8482,20 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="545" t="s">
         <v>314</v>
       </c>
-      <c r="B2" s="540"/>
-      <c r="C2" s="540"/>
-      <c r="D2" s="540"/>
-      <c r="E2" s="540"/>
-      <c r="F2" s="540"/>
-      <c r="G2" s="540"/>
-      <c r="H2" s="540"/>
-      <c r="I2" s="540"/>
-      <c r="J2" s="540"/>
-      <c r="K2" s="540"/>
-      <c r="L2" s="540"/>
+      <c r="B2" s="545"/>
+      <c r="C2" s="545"/>
+      <c r="D2" s="545"/>
+      <c r="E2" s="545"/>
+      <c r="F2" s="545"/>
+      <c r="G2" s="545"/>
+      <c r="H2" s="545"/>
+      <c r="I2" s="545"/>
+      <c r="J2" s="545"/>
+      <c r="K2" s="545"/>
+      <c r="L2" s="545"/>
     </row>
     <row r="3" spans="1:15" s="15" customFormat="1" ht="180" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="329" t="s">
@@ -8600,28 +8635,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L2"/>
+  <autoFilter ref="A1:L2" xr:uid="{00000000-0009-0000-0000-00000B000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="70" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="50" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="A5" sqref="A5"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="76" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="39" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="70" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="G5" sqref="G5"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="39" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="50" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="A5" sqref="A5"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="70" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="39" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="76" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -8630,7 +8665,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H4" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -8643,15 +8678,15 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
     <tabColor indexed="50"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8668,32 +8703,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="545" t="s">
+      <c r="A1" s="550" t="s">
         <v>317</v>
       </c>
-      <c r="B1" s="545"/>
-      <c r="C1" s="545"/>
-      <c r="D1" s="545"/>
-      <c r="E1" s="545"/>
-      <c r="F1" s="545"/>
-      <c r="G1" s="545"/>
-      <c r="H1" s="545"/>
-      <c r="I1" s="545"/>
-      <c r="J1" s="545"/>
+      <c r="B1" s="550"/>
+      <c r="C1" s="550"/>
+      <c r="D1" s="550"/>
+      <c r="E1" s="550"/>
+      <c r="F1" s="550"/>
+      <c r="G1" s="550"/>
+      <c r="H1" s="550"/>
+      <c r="I1" s="550"/>
+      <c r="J1" s="550"/>
     </row>
     <row r="2" spans="1:10" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="546" t="s">
+      <c r="A2" s="551" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="546"/>
-      <c r="C2" s="546"/>
-      <c r="D2" s="546"/>
-      <c r="E2" s="546"/>
-      <c r="F2" s="546"/>
-      <c r="G2" s="546"/>
-      <c r="H2" s="546"/>
-      <c r="I2" s="546"/>
-      <c r="J2" s="546"/>
+      <c r="B2" s="551"/>
+      <c r="C2" s="551"/>
+      <c r="D2" s="551"/>
+      <c r="E2" s="551"/>
+      <c r="F2" s="551"/>
+      <c r="G2" s="551"/>
+      <c r="H2" s="551"/>
+      <c r="I2" s="551"/>
+      <c r="J2" s="551"/>
     </row>
     <row r="3" spans="1:10" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="412"/>
@@ -8729,27 +8764,27 @@
       <c r="G4" s="411" t="s">
         <v>340</v>
       </c>
-      <c r="H4" s="529" t="s">
+      <c r="H4" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="I4" s="529"/>
+      <c r="I4" s="534"/>
       <c r="J4" s="445" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="543" t="s">
+      <c r="A5" s="548" t="s">
         <v>319</v>
       </c>
-      <c r="B5" s="543"/>
-      <c r="C5" s="543"/>
-      <c r="D5" s="543"/>
-      <c r="E5" s="543"/>
-      <c r="F5" s="543"/>
-      <c r="G5" s="543"/>
-      <c r="H5" s="543"/>
-      <c r="I5" s="543"/>
-      <c r="J5" s="543"/>
+      <c r="B5" s="548"/>
+      <c r="C5" s="548"/>
+      <c r="D5" s="548"/>
+      <c r="E5" s="548"/>
+      <c r="F5" s="548"/>
+      <c r="G5" s="548"/>
+      <c r="H5" s="548"/>
+      <c r="I5" s="548"/>
+      <c r="J5" s="548"/>
     </row>
     <row r="6" spans="1:10" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="458" t="s">
@@ -8935,18 +8970,18 @@
       <c r="J11" s="131"/>
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="543" t="s">
+      <c r="A12" s="548" t="s">
         <v>1195</v>
       </c>
-      <c r="B12" s="543"/>
-      <c r="C12" s="543"/>
-      <c r="D12" s="543"/>
-      <c r="E12" s="543"/>
-      <c r="F12" s="543"/>
-      <c r="G12" s="543"/>
-      <c r="H12" s="543"/>
-      <c r="I12" s="543"/>
-      <c r="J12" s="543"/>
+      <c r="B12" s="548"/>
+      <c r="C12" s="548"/>
+      <c r="D12" s="548"/>
+      <c r="E12" s="548"/>
+      <c r="F12" s="548"/>
+      <c r="G12" s="548"/>
+      <c r="H12" s="548"/>
+      <c r="I12" s="548"/>
+      <c r="J12" s="548"/>
     </row>
     <row r="13" spans="1:10" s="129" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="458" t="s">
@@ -9244,18 +9279,18 @@
       <c r="J21" s="131"/>
     </row>
     <row r="22" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="543" t="s">
+      <c r="A22" s="548" t="s">
         <v>320</v>
       </c>
-      <c r="B22" s="543"/>
-      <c r="C22" s="543"/>
-      <c r="D22" s="543"/>
-      <c r="E22" s="543"/>
-      <c r="F22" s="543"/>
-      <c r="G22" s="543"/>
-      <c r="H22" s="543"/>
-      <c r="I22" s="543"/>
-      <c r="J22" s="543"/>
+      <c r="B22" s="548"/>
+      <c r="C22" s="548"/>
+      <c r="D22" s="548"/>
+      <c r="E22" s="548"/>
+      <c r="F22" s="548"/>
+      <c r="G22" s="548"/>
+      <c r="H22" s="548"/>
+      <c r="I22" s="548"/>
+      <c r="J22" s="548"/>
     </row>
     <row r="23" spans="1:10" s="129" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A23" s="458" t="s">
@@ -9449,18 +9484,18 @@
       <c r="J28" s="131"/>
     </row>
     <row r="29" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A29" s="544" t="s">
+      <c r="A29" s="549" t="s">
         <v>321</v>
       </c>
-      <c r="B29" s="544"/>
-      <c r="C29" s="544"/>
-      <c r="D29" s="544"/>
-      <c r="E29" s="544"/>
-      <c r="F29" s="544"/>
-      <c r="G29" s="544"/>
-      <c r="H29" s="544"/>
-      <c r="I29" s="544"/>
-      <c r="J29" s="544"/>
+      <c r="B29" s="549"/>
+      <c r="C29" s="549"/>
+      <c r="D29" s="549"/>
+      <c r="E29" s="549"/>
+      <c r="F29" s="549"/>
+      <c r="G29" s="549"/>
+      <c r="H29" s="549"/>
+      <c r="I29" s="549"/>
+      <c r="J29" s="549"/>
     </row>
     <row r="30" spans="1:10" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="130"/>
@@ -10579,28 +10614,28 @@
       <c r="J123" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:J30"/>
+  <autoFilter ref="A4:J30" xr:uid="{00000000-0009-0000-0000-00000C000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="72" fitToPage="1" showAutoFilter="1">
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="72" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="D4" sqref="D4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="87" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="49" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:K1"/>
+      <autoFilter ref="B1:K1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="72" fitToPage="1" showAutoFilter="1">
       <selection activeCell="D4" sqref="D4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="49" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:K1"/>
+      <autoFilter ref="B1:K1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="72" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="72" fitToPage="1" showAutoFilter="1">
       <selection activeCell="D4" sqref="D4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="49" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="87" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:K1"/>
+      <autoFilter ref="B1:K1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="7">
@@ -10614,7 +10649,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G10 G13:G20">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G10 G13:G20" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -10627,14 +10662,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10648,31 +10683,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="15" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="541" t="s">
+      <c r="A1" s="546" t="s">
         <v>322</v>
       </c>
-      <c r="B1" s="541"/>
-      <c r="C1" s="541"/>
-      <c r="D1" s="541"/>
-      <c r="E1" s="541"/>
-      <c r="F1" s="541"/>
-      <c r="G1" s="541"/>
-      <c r="H1" s="541"/>
-      <c r="I1" s="541"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
       <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" s="15" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="542" t="s">
+      <c r="A2" s="547" t="s">
         <v>318</v>
       </c>
-      <c r="B2" s="542"/>
-      <c r="C2" s="542"/>
-      <c r="D2" s="542"/>
-      <c r="E2" s="542"/>
-      <c r="F2" s="542"/>
-      <c r="G2" s="542"/>
-      <c r="H2" s="542"/>
-      <c r="I2" s="542"/>
+      <c r="B2" s="547"/>
+      <c r="C2" s="547"/>
+      <c r="D2" s="547"/>
+      <c r="E2" s="547"/>
+      <c r="F2" s="547"/>
+      <c r="G2" s="547"/>
+      <c r="H2" s="547"/>
+      <c r="I2" s="547"/>
       <c r="J2" s="26"/>
     </row>
     <row r="3" spans="1:10" s="15" customFormat="1" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -10706,26 +10741,26 @@
       <c r="F4" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="G4" s="532" t="s">
+      <c r="G4" s="537" t="s">
         <v>341</v>
       </c>
-      <c r="H4" s="532"/>
+      <c r="H4" s="537"/>
       <c r="I4" s="23" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="543" t="s">
+      <c r="A5" s="548" t="s">
         <v>1195</v>
       </c>
-      <c r="B5" s="543"/>
-      <c r="C5" s="543"/>
-      <c r="D5" s="543"/>
-      <c r="E5" s="543"/>
-      <c r="F5" s="543"/>
-      <c r="G5" s="543"/>
-      <c r="H5" s="543"/>
-      <c r="I5" s="543"/>
+      <c r="B5" s="548"/>
+      <c r="C5" s="548"/>
+      <c r="D5" s="548"/>
+      <c r="E5" s="548"/>
+      <c r="F5" s="548"/>
+      <c r="G5" s="548"/>
+      <c r="H5" s="548"/>
+      <c r="I5" s="548"/>
       <c r="J5" s="29"/>
     </row>
     <row r="6" spans="1:10" s="129" customFormat="1" ht="60" x14ac:dyDescent="0.2">
@@ -10836,28 +10871,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:I8"/>
+  <autoFilter ref="A4:I8" xr:uid="{00000000-0009-0000-0000-00000D000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="90" fitToPage="1" showAutoFilter="1">
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="53" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:J1"/>
+      <autoFilter ref="B1:J1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="90" fitToPage="1" showAutoFilter="1">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="53" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:J1"/>
+      <autoFilter ref="B1:J1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="90" fitToPage="1" showAutoFilter="1">
       <selection activeCell="C4" sqref="C4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="53" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:J1"/>
+      <autoFilter ref="B1:J1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="4">
@@ -10868,7 +10903,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F7" xr:uid="{00000000-0002-0000-0D00-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -10881,7 +10916,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <sheetPr>
     <tabColor indexed="51"/>
     <pageSetUpPr fitToPage="1"/>
@@ -10889,7 +10924,7 @@
   <dimension ref="A1:O39"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="81" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I4" sqref="I4:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10910,36 +10945,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="15" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="541" t="s">
+      <c r="A1" s="546" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="541"/>
-      <c r="C1" s="541"/>
-      <c r="D1" s="541"/>
-      <c r="E1" s="541"/>
-      <c r="F1" s="541"/>
-      <c r="G1" s="541"/>
-      <c r="H1" s="541"/>
-      <c r="I1" s="541"/>
-      <c r="J1" s="541"/>
-      <c r="K1" s="541"/>
-      <c r="L1" s="541"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
+      <c r="K1" s="546"/>
+      <c r="L1" s="546"/>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="542" t="s">
+      <c r="A2" s="547" t="s">
         <v>325</v>
       </c>
-      <c r="B2" s="542"/>
-      <c r="C2" s="542"/>
-      <c r="D2" s="542"/>
-      <c r="E2" s="542"/>
-      <c r="F2" s="542"/>
-      <c r="G2" s="542"/>
-      <c r="H2" s="542"/>
-      <c r="I2" s="542"/>
-      <c r="J2" s="542"/>
-      <c r="K2" s="542"/>
-      <c r="L2" s="542"/>
+      <c r="B2" s="547"/>
+      <c r="C2" s="547"/>
+      <c r="D2" s="547"/>
+      <c r="E2" s="547"/>
+      <c r="F2" s="547"/>
+      <c r="G2" s="547"/>
+      <c r="H2" s="547"/>
+      <c r="I2" s="547"/>
+      <c r="J2" s="547"/>
+      <c r="K2" s="547"/>
+      <c r="L2" s="547"/>
     </row>
     <row r="3" spans="1:15" s="15" customFormat="1" ht="3" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59"/>
@@ -10980,10 +11015,10 @@
       <c r="H4" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="I4" s="529" t="s">
+      <c r="I4" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="J4" s="529"/>
+      <c r="J4" s="534"/>
       <c r="K4" s="61" t="s">
         <v>2</v>
       </c>
@@ -11001,20 +11036,20 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="6" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="535" t="s">
+      <c r="A5" s="540" t="s">
         <v>323</v>
       </c>
-      <c r="B5" s="535"/>
-      <c r="C5" s="535"/>
-      <c r="D5" s="535"/>
-      <c r="E5" s="535"/>
-      <c r="F5" s="535"/>
-      <c r="G5" s="535"/>
-      <c r="H5" s="535"/>
-      <c r="I5" s="535"/>
-      <c r="J5" s="535"/>
-      <c r="K5" s="535"/>
-      <c r="L5" s="535"/>
+      <c r="B5" s="540"/>
+      <c r="C5" s="540"/>
+      <c r="D5" s="540"/>
+      <c r="E5" s="540"/>
+      <c r="F5" s="540"/>
+      <c r="G5" s="540"/>
+      <c r="H5" s="540"/>
+      <c r="I5" s="540"/>
+      <c r="J5" s="540"/>
+      <c r="K5" s="540"/>
+      <c r="L5" s="540"/>
     </row>
     <row r="6" spans="1:15" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="137" t="s">
@@ -12517,28 +12552,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:L37"/>
+  <autoFilter ref="A4:L37" xr:uid="{00000000-0009-0000-0000-00000E000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D4" sqref="D4"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="F10" sqref="F10"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="89" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="51" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="80" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="L4" sqref="L4:P4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="51" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="F10" sqref="F10"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D4" sqref="D4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="51" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="89" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="4">
@@ -12549,7 +12584,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H37">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H37" xr:uid="{00000000-0002-0000-0E00-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -12562,8 +12597,8 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
     <tabColor indexed="51"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -12615,10 +12650,10 @@
       <c r="G1" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="H1" s="529" t="s">
+      <c r="H1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="I1" s="529"/>
+      <c r="I1" s="534"/>
       <c r="J1" s="61" t="s">
         <v>2</v>
       </c>
@@ -12636,19 +12671,19 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="6" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="535" t="s">
+      <c r="A2" s="540" t="s">
         <v>326</v>
       </c>
-      <c r="B2" s="535"/>
-      <c r="C2" s="535"/>
-      <c r="D2" s="535"/>
-      <c r="E2" s="535"/>
-      <c r="F2" s="535"/>
-      <c r="G2" s="535"/>
-      <c r="H2" s="535"/>
-      <c r="I2" s="535"/>
-      <c r="J2" s="535"/>
-      <c r="K2" s="535"/>
+      <c r="B2" s="540"/>
+      <c r="C2" s="540"/>
+      <c r="D2" s="540"/>
+      <c r="E2" s="540"/>
+      <c r="F2" s="540"/>
+      <c r="G2" s="540"/>
+      <c r="H2" s="540"/>
+      <c r="I2" s="540"/>
+      <c r="J2" s="540"/>
+      <c r="K2" s="540"/>
       <c r="N2" s="166"/>
     </row>
     <row r="3" spans="1:14" s="5" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -12936,28 +12971,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K10"/>
+  <autoFilter ref="A1:K10" xr:uid="{00000000-0009-0000-0000-00000F000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="D12" sqref="D12"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="94" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="61" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="L1" sqref="L1:P1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="61" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="D12" sqref="D12"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="61" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="94" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -12966,7 +13001,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G8" xr:uid="{00000000-0002-0000-0F00-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -12980,15 +13015,15 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
     <tabColor indexed="51"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:K2"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -13025,15 +13060,15 @@
         <v>1136</v>
       </c>
       <c r="F1" s="65" t="s">
-        <v>1236</v>
+        <v>339</v>
       </c>
       <c r="G1" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="H1" s="529" t="s">
+      <c r="H1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="I1" s="529"/>
+      <c r="I1" s="534"/>
       <c r="J1" s="61" t="s">
         <v>2</v>
       </c>
@@ -13051,19 +13086,19 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="535" t="s">
+      <c r="A2" s="540" t="s">
         <v>327</v>
       </c>
-      <c r="B2" s="535"/>
-      <c r="C2" s="535"/>
-      <c r="D2" s="535"/>
-      <c r="E2" s="535"/>
-      <c r="F2" s="535"/>
-      <c r="G2" s="535"/>
-      <c r="H2" s="535"/>
-      <c r="I2" s="535"/>
-      <c r="J2" s="535"/>
-      <c r="K2" s="535"/>
+      <c r="B2" s="540"/>
+      <c r="C2" s="540"/>
+      <c r="D2" s="540"/>
+      <c r="E2" s="540"/>
+      <c r="F2" s="540"/>
+      <c r="G2" s="540"/>
+      <c r="H2" s="540"/>
+      <c r="I2" s="540"/>
+      <c r="J2" s="540"/>
+      <c r="K2" s="540"/>
       <c r="L2" s="392"/>
     </row>
     <row r="3" spans="1:14" s="126" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
@@ -14062,28 +14097,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K29"/>
+  <autoFilter ref="A1:K29" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="90" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" topLeftCell="A16">
+      <selection activeCell="E24" sqref="E24"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="90" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="54" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="90" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="L6" sqref="L6"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="54" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" topLeftCell="A16">
-      <selection activeCell="E24" sqref="E24"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="90" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="54" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="90" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -14092,7 +14127,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G28">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G28" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -14105,15 +14140,15 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
     <tabColor indexed="51"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O82"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14154,10 +14189,10 @@
       <c r="G1" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="H1" s="529" t="s">
+      <c r="H1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="I1" s="529"/>
+      <c r="I1" s="534"/>
       <c r="J1" s="61" t="s">
         <v>2</v>
       </c>
@@ -14176,19 +14211,19 @@
       <c r="O1" s="89"/>
     </row>
     <row r="2" spans="1:15" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="535" t="s">
+      <c r="A2" s="540" t="s">
         <v>328</v>
       </c>
-      <c r="B2" s="535"/>
-      <c r="C2" s="535"/>
-      <c r="D2" s="535"/>
-      <c r="E2" s="535"/>
-      <c r="F2" s="535"/>
-      <c r="G2" s="535"/>
-      <c r="H2" s="535"/>
-      <c r="I2" s="535"/>
-      <c r="J2" s="535"/>
-      <c r="K2" s="535"/>
+      <c r="B2" s="540"/>
+      <c r="C2" s="540"/>
+      <c r="D2" s="540"/>
+      <c r="E2" s="540"/>
+      <c r="F2" s="540"/>
+      <c r="G2" s="540"/>
+      <c r="H2" s="540"/>
+      <c r="I2" s="540"/>
+      <c r="J2" s="540"/>
+      <c r="K2" s="540"/>
       <c r="L2" s="391"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -17567,32 +17602,32 @@
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C82" s="158" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K75"/>
+  <autoFilter ref="A1:K75" xr:uid="{00000000-0009-0000-0000-000011000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="90" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" topLeftCell="A49">
+      <selection activeCell="A39" sqref="A39"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="87" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="51" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="90" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="P3" sqref="P3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="51" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" topLeftCell="A49">
-      <selection activeCell="A39" sqref="A39"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="90" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="51" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="87" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -17601,7 +17636,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G75">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G75" xr:uid="{00000000-0002-0000-1100-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -17614,8 +17649,8 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
     <tabColor indexed="51"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -17643,35 +17678,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="15" customFormat="1" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="541" t="s">
+      <c r="A1" s="546" t="s">
         <v>329</v>
       </c>
-      <c r="B1" s="541"/>
-      <c r="C1" s="541"/>
-      <c r="D1" s="541"/>
-      <c r="E1" s="541"/>
-      <c r="F1" s="541"/>
-      <c r="G1" s="541"/>
-      <c r="H1" s="541"/>
-      <c r="I1" s="541"/>
-      <c r="J1" s="541"/>
-      <c r="K1" s="541"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
+      <c r="K1" s="546"/>
       <c r="N1" s="421"/>
     </row>
     <row r="2" spans="1:15" s="15" customFormat="1" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="542" t="s">
+      <c r="A2" s="547" t="s">
         <v>325</v>
       </c>
-      <c r="B2" s="542"/>
-      <c r="C2" s="542"/>
-      <c r="D2" s="542"/>
-      <c r="E2" s="542"/>
-      <c r="F2" s="542"/>
-      <c r="G2" s="542"/>
-      <c r="H2" s="542"/>
-      <c r="I2" s="542"/>
-      <c r="J2" s="542"/>
-      <c r="K2" s="542"/>
+      <c r="B2" s="547"/>
+      <c r="C2" s="547"/>
+      <c r="D2" s="547"/>
+      <c r="E2" s="547"/>
+      <c r="F2" s="547"/>
+      <c r="G2" s="547"/>
+      <c r="H2" s="547"/>
+      <c r="I2" s="547"/>
+      <c r="J2" s="547"/>
+      <c r="K2" s="547"/>
       <c r="N2" s="421"/>
     </row>
     <row r="3" spans="1:15" s="15" customFormat="1" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -17710,10 +17745,10 @@
       <c r="G4" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="H4" s="529" t="s">
+      <c r="H4" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="I4" s="529"/>
+      <c r="I4" s="534"/>
       <c r="J4" s="73" t="s">
         <v>2</v>
       </c>
@@ -17731,19 +17766,19 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="540" t="s">
+      <c r="A5" s="545" t="s">
         <v>323</v>
       </c>
-      <c r="B5" s="540"/>
-      <c r="C5" s="540"/>
-      <c r="D5" s="540"/>
-      <c r="E5" s="540"/>
-      <c r="F5" s="540"/>
-      <c r="G5" s="540"/>
-      <c r="H5" s="540"/>
-      <c r="I5" s="540"/>
-      <c r="J5" s="540"/>
-      <c r="K5" s="540"/>
+      <c r="B5" s="545"/>
+      <c r="C5" s="545"/>
+      <c r="D5" s="545"/>
+      <c r="E5" s="545"/>
+      <c r="F5" s="545"/>
+      <c r="G5" s="545"/>
+      <c r="H5" s="545"/>
+      <c r="I5" s="545"/>
+      <c r="J5" s="545"/>
+      <c r="K5" s="545"/>
     </row>
     <row r="6" spans="1:15" s="129" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="284" t="s">
@@ -18279,28 +18314,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:K17"/>
+  <autoFilter ref="A4:K17" xr:uid="{00000000-0009-0000-0000-000012000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="90" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D4" sqref="D4"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" topLeftCell="B1">
+      <selection activeCell="B6" sqref="B6:L6"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="90" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="52" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="90" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="P5" sqref="P5"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="52" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" topLeftCell="B1">
-      <selection activeCell="B6" sqref="B6:L6"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="90" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D4" sqref="D4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="52" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="90" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="4">
@@ -18311,7 +18346,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G17" xr:uid="{00000000-0002-0000-1200-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -18324,13 +18359,13 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -18375,10 +18410,10 @@
       <c r="H1" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="532" t="s">
+      <c r="I1" s="537" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="532"/>
+      <c r="J1" s="537"/>
       <c r="K1" s="11" t="s">
         <v>2</v>
       </c>
@@ -18396,20 +18431,20 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="6" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="533" t="s">
+      <c r="A2" s="538" t="s">
         <v>311</v>
       </c>
-      <c r="B2" s="533"/>
-      <c r="C2" s="533"/>
-      <c r="D2" s="533"/>
-      <c r="E2" s="533"/>
-      <c r="F2" s="533"/>
-      <c r="G2" s="533"/>
-      <c r="H2" s="533"/>
-      <c r="I2" s="533"/>
-      <c r="J2" s="533"/>
-      <c r="K2" s="533"/>
-      <c r="L2" s="533"/>
+      <c r="B2" s="538"/>
+      <c r="C2" s="538"/>
+      <c r="D2" s="538"/>
+      <c r="E2" s="538"/>
+      <c r="F2" s="538"/>
+      <c r="G2" s="538"/>
+      <c r="H2" s="538"/>
+      <c r="I2" s="538"/>
+      <c r="J2" s="538"/>
+      <c r="K2" s="538"/>
+      <c r="L2" s="538"/>
       <c r="O2" s="166"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.2">
@@ -18570,28 +18605,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L5"/>
+  <autoFilter ref="A1:L5" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="50" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="L3" sqref="L3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="48" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="80" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="P3" sqref="P3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="49" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="50" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="L3" sqref="L3"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="48" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -18600,7 +18635,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H5" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -18614,15 +18649,15 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
     <tabColor indexed="51"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView zoomScale="101" zoomScaleNormal="101" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18630,9 +18665,9 @@
     <col min="1" max="1" width="18.5703125" style="2" customWidth="1"/>
     <col min="2" max="2" width="17" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="45" hidden="1" customWidth="1"/>
-    <col min="6" max="10" width="16.42578125" style="45" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="2" customWidth="1"/>
+    <col min="5" max="7" width="25.28515625" style="45" customWidth="1"/>
+    <col min="8" max="10" width="16.42578125" style="45" customWidth="1"/>
     <col min="11" max="11" width="9" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16.7109375" style="1" customWidth="1"/>
@@ -18666,10 +18701,10 @@
       <c r="H1" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="529" t="s">
+      <c r="I1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="529"/>
+      <c r="J1" s="534"/>
       <c r="K1" s="73" t="s">
         <v>2</v>
       </c>
@@ -18688,20 +18723,20 @@
       <c r="P1" s="91"/>
     </row>
     <row r="2" spans="1:16" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="545" t="s">
         <v>326</v>
       </c>
-      <c r="B2" s="540"/>
-      <c r="C2" s="540"/>
-      <c r="D2" s="540"/>
-      <c r="E2" s="540"/>
-      <c r="F2" s="540"/>
-      <c r="G2" s="540"/>
-      <c r="H2" s="540"/>
-      <c r="I2" s="540"/>
-      <c r="J2" s="540"/>
-      <c r="K2" s="540"/>
-      <c r="L2" s="540"/>
+      <c r="B2" s="545"/>
+      <c r="C2" s="545"/>
+      <c r="D2" s="545"/>
+      <c r="E2" s="545"/>
+      <c r="F2" s="545"/>
+      <c r="G2" s="545"/>
+      <c r="H2" s="545"/>
+      <c r="I2" s="545"/>
+      <c r="J2" s="545"/>
+      <c r="K2" s="545"/>
+      <c r="L2" s="545"/>
       <c r="P2" s="90"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -18904,28 +18939,28 @@
       <c r="D26" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L3"/>
+  <autoFilter ref="A1:L3" xr:uid="{00000000-0009-0000-0000-000013000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="73" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="73" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="I34" sqref="I34"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="94" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="57" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="73" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="P3" sqref="P3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="57" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="73" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="I34" sqref="I34"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="73" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="57" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="94" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -18934,7 +18969,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H6" xr:uid="{00000000-0002-0000-1300-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -18947,8 +18982,8 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
     <tabColor indexed="51"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -18996,10 +19031,10 @@
       <c r="G1" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="H1" s="529" t="s">
+      <c r="H1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="I1" s="529"/>
+      <c r="I1" s="534"/>
       <c r="J1" s="73" t="s">
         <v>2</v>
       </c>
@@ -19018,19 +19053,22 @@
       <c r="O1" s="88"/>
     </row>
     <row r="2" spans="1:15" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="545" t="s">
         <v>327</v>
       </c>
-      <c r="B2" s="540"/>
-      <c r="C2" s="540"/>
-      <c r="D2" s="540"/>
-      <c r="E2" s="540"/>
-      <c r="F2" s="540"/>
-      <c r="G2" s="540"/>
-      <c r="H2" s="540"/>
-      <c r="I2" s="540"/>
-      <c r="J2" s="540"/>
-      <c r="K2" s="540"/>
+      <c r="B2" s="545"/>
+      <c r="C2" s="545"/>
+      <c r="D2" s="545"/>
+      <c r="E2" s="545"/>
+      <c r="F2" s="545"/>
+      <c r="G2" s="545"/>
+      <c r="H2" s="545"/>
+      <c r="I2" s="545"/>
+      <c r="J2" s="545"/>
+      <c r="K2" s="545"/>
+      <c r="L2" s="421" t="s">
+        <v>1243</v>
+      </c>
     </row>
     <row r="3" spans="1:15" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="69" t="s">
@@ -19150,28 +19188,28 @@
       <c r="I7" s="41"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K5"/>
+  <autoFilter ref="A1:K5" xr:uid="{00000000-0009-0000-0000-000014000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="D17" sqref="D17"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="94" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="57" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="M4" sqref="M4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="57" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="D17" sqref="D17"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="57" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="94" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -19180,7 +19218,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G5" xr:uid="{00000000-0002-0000-1400-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -19193,8 +19231,8 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <sheetPr>
     <tabColor indexed="51"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -19242,10 +19280,10 @@
       <c r="G1" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="H1" s="529" t="s">
+      <c r="H1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="I1" s="529"/>
+      <c r="I1" s="534"/>
       <c r="J1" s="73" t="s">
         <v>2</v>
       </c>
@@ -19264,19 +19302,19 @@
       <c r="O1" s="88"/>
     </row>
     <row r="2" spans="1:15" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="540" t="s">
+      <c r="A2" s="545" t="s">
         <v>328</v>
       </c>
-      <c r="B2" s="540"/>
-      <c r="C2" s="540"/>
-      <c r="D2" s="540"/>
-      <c r="E2" s="540"/>
-      <c r="F2" s="540"/>
-      <c r="G2" s="540"/>
-      <c r="H2" s="540"/>
-      <c r="I2" s="540"/>
-      <c r="J2" s="540"/>
-      <c r="K2" s="540"/>
+      <c r="B2" s="545"/>
+      <c r="C2" s="545"/>
+      <c r="D2" s="545"/>
+      <c r="E2" s="545"/>
+      <c r="F2" s="545"/>
+      <c r="G2" s="545"/>
+      <c r="H2" s="545"/>
+      <c r="I2" s="545"/>
+      <c r="J2" s="545"/>
+      <c r="K2" s="545"/>
     </row>
     <row r="3" spans="1:15" s="15" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="297" t="s">
@@ -19463,28 +19501,28 @@
       <c r="I10" s="41"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K6"/>
+  <autoFilter ref="A1:K6" xr:uid="{00000000-0009-0000-0000-000015000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="90" fitToPage="1" showAutoFilter="1">
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="90" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="52" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="90" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="P3" sqref="P3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="52" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="90" fitToPage="1" showAutoFilter="1">
       <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="52" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="90" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -19493,7 +19531,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G6" xr:uid="{00000000-0002-0000-1500-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -19506,7 +19544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -19607,7 +19645,8 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}">
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}">
+      <selection activeCell="D15" sqref="D14:D15"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId1"/>
       <headerFooter alignWithMargins="0">
@@ -19622,8 +19661,7 @@
         <oddFooter>&amp;R&amp;"Arial,Italic"&amp;8&amp;Z&amp;F</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}">
-      <selection activeCell="D15" sqref="D14:D15"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}">
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" r:id="rId3"/>
       <headerFooter alignWithMargins="0">
@@ -19632,7 +19670,7 @@
     </customSheetView>
   </customSheetViews>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G14" xr:uid="{00000000-0002-0000-1600-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -19646,13 +19684,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
@@ -19698,10 +19736,10 @@
       <c r="H1" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="532" t="s">
+      <c r="I1" s="537" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="532"/>
+      <c r="J1" s="537"/>
       <c r="K1" s="13" t="s">
         <v>2</v>
       </c>
@@ -19719,25 +19757,25 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="6" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="534" t="s">
+      <c r="A2" s="539" t="s">
         <v>312</v>
       </c>
-      <c r="B2" s="534"/>
-      <c r="C2" s="534"/>
-      <c r="D2" s="534"/>
-      <c r="E2" s="534"/>
-      <c r="F2" s="534"/>
-      <c r="G2" s="534"/>
-      <c r="H2" s="534"/>
-      <c r="I2" s="534"/>
-      <c r="J2" s="534"/>
-      <c r="K2" s="534"/>
-      <c r="L2" s="534"/>
+      <c r="B2" s="539"/>
+      <c r="C2" s="539"/>
+      <c r="D2" s="539"/>
+      <c r="E2" s="539"/>
+      <c r="F2" s="539"/>
+      <c r="G2" s="539"/>
+      <c r="H2" s="539"/>
+      <c r="I2" s="539"/>
+      <c r="J2" s="539"/>
+      <c r="K2" s="539"/>
+      <c r="L2" s="539"/>
       <c r="O2" s="166"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" ht="90" x14ac:dyDescent="0.2">
       <c r="A3" s="112" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="B3" s="112" t="s">
         <v>120</v>
@@ -19778,8 +19816,8 @@
         <v>1147</v>
       </c>
       <c r="N3" s="82"/>
-      <c r="O3" s="547" t="s">
-        <v>1238</v>
+      <c r="O3" s="527" t="s">
+        <v>1237</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.2">
@@ -20858,28 +20896,28 @@
       <c r="N27" s="97"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L23"/>
+  <autoFilter ref="A1:L23" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="50" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="B37" sqref="B37"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="81" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="50" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="80" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="P3" sqref="P3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="51" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="50" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="B37" sqref="B37"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="50" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="81" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -20888,7 +20926,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H25" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -20902,14 +20940,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -20954,10 +20992,10 @@
       <c r="H1" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="529" t="s">
+      <c r="I1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="529"/>
+      <c r="J1" s="534"/>
       <c r="K1" s="61" t="s">
         <v>2</v>
       </c>
@@ -20976,20 +21014,20 @@
       <c r="P1" s="89"/>
     </row>
     <row r="2" spans="1:16" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="535" t="s">
+      <c r="A2" s="540" t="s">
         <v>313</v>
       </c>
-      <c r="B2" s="535"/>
-      <c r="C2" s="535"/>
-      <c r="D2" s="535"/>
-      <c r="E2" s="535"/>
-      <c r="F2" s="535"/>
-      <c r="G2" s="535"/>
-      <c r="H2" s="535"/>
-      <c r="I2" s="535"/>
-      <c r="J2" s="535"/>
-      <c r="K2" s="535"/>
-      <c r="L2" s="535"/>
+      <c r="B2" s="540"/>
+      <c r="C2" s="540"/>
+      <c r="D2" s="540"/>
+      <c r="E2" s="540"/>
+      <c r="F2" s="540"/>
+      <c r="G2" s="540"/>
+      <c r="H2" s="540"/>
+      <c r="I2" s="540"/>
+      <c r="J2" s="540"/>
+      <c r="K2" s="540"/>
+      <c r="L2" s="540"/>
     </row>
     <row r="3" spans="1:16" s="83" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="113" t="s">
@@ -22405,28 +22443,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L31"/>
+  <autoFilter ref="A1:L31" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="81" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="51" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="80" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="51" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="D11" sqref="D11"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="51" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="81" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -22435,7 +22473,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H31" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -22449,13 +22487,13 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -22501,10 +22539,10 @@
       <c r="H1" s="161" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="529" t="s">
+      <c r="I1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="529"/>
+      <c r="J1" s="534"/>
       <c r="K1" s="163" t="s">
         <v>2</v>
       </c>
@@ -22522,20 +22560,20 @@
       </c>
     </row>
     <row r="2" spans="1:15" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="536" t="s">
+      <c r="A2" s="541" t="s">
         <v>314</v>
       </c>
-      <c r="B2" s="536"/>
-      <c r="C2" s="536"/>
-      <c r="D2" s="536"/>
-      <c r="E2" s="536"/>
-      <c r="F2" s="536"/>
-      <c r="G2" s="536"/>
-      <c r="H2" s="536"/>
-      <c r="I2" s="536"/>
-      <c r="J2" s="536"/>
-      <c r="K2" s="536"/>
-      <c r="L2" s="536"/>
+      <c r="B2" s="541"/>
+      <c r="C2" s="541"/>
+      <c r="D2" s="541"/>
+      <c r="E2" s="541"/>
+      <c r="F2" s="541"/>
+      <c r="G2" s="541"/>
+      <c r="H2" s="541"/>
+      <c r="I2" s="541"/>
+      <c r="J2" s="541"/>
+      <c r="K2" s="541"/>
+      <c r="L2" s="541"/>
       <c r="M2" s="241"/>
       <c r="N2" s="241"/>
       <c r="O2" s="241"/>
@@ -22990,7 +23028,7 @@
       </c>
       <c r="O12" s="152"/>
     </row>
-    <row r="13" spans="1:15" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A13" s="112" t="s">
         <v>105</v>
       </c>
@@ -23456,7 +23494,7 @@
       </c>
       <c r="O22" s="245"/>
     </row>
-    <row r="23" spans="1:15" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:15" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A23" s="112" t="s">
         <v>93</v>
       </c>
@@ -24672,14 +24710,14 @@
       <c r="K49" s="510"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L47"/>
+  <autoFilter ref="A1:L47" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="75" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="C13" sqref="C13"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="49" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="80" fitToPage="1" printArea="1" showAutoFilter="1">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
@@ -24687,14 +24725,14 @@
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="49" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="75" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="C13" sqref="C13"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="49" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -24703,7 +24741,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H16:H47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H16:H47" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -24717,7 +24755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -24765,10 +24803,10 @@
       <c r="G1" s="65" t="s">
         <v>1215</v>
       </c>
-      <c r="H1" s="529" t="s">
+      <c r="H1" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="I1" s="529"/>
+      <c r="I1" s="534"/>
       <c r="J1" s="61" t="s">
         <v>2</v>
       </c>
@@ -24783,19 +24821,19 @@
       </c>
     </row>
     <row r="2" spans="1:14" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="537" t="s">
+      <c r="A2" s="542" t="s">
         <v>315</v>
       </c>
-      <c r="B2" s="538"/>
-      <c r="C2" s="538"/>
-      <c r="D2" s="538"/>
-      <c r="E2" s="538"/>
-      <c r="F2" s="538"/>
-      <c r="G2" s="538"/>
-      <c r="H2" s="538"/>
-      <c r="I2" s="538"/>
-      <c r="J2" s="538"/>
-      <c r="K2" s="539"/>
+      <c r="B2" s="543"/>
+      <c r="C2" s="543"/>
+      <c r="D2" s="543"/>
+      <c r="E2" s="543"/>
+      <c r="F2" s="543"/>
+      <c r="G2" s="543"/>
+      <c r="H2" s="543"/>
+      <c r="I2" s="543"/>
+      <c r="J2" s="543"/>
+      <c r="K2" s="544"/>
     </row>
     <row r="3" spans="1:14" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.2">
       <c r="A3" s="327" t="s">
@@ -25849,28 +25887,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K28"/>
+  <autoFilter ref="A1:K28" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D1" sqref="D1"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" topLeftCell="A4">
+      <selection activeCell="C21" sqref="C21"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="81" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="51" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="80" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="C14" sqref="C14"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="51" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1" topLeftCell="A4">
-      <selection activeCell="C21" sqref="C21"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="51" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="81" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -25879,7 +25917,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G27">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G27" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -25892,14 +25930,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25942,10 +25980,10 @@
       <c r="H1" s="35" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="532" t="s">
+      <c r="I1" s="537" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="532"/>
+      <c r="J1" s="537"/>
       <c r="K1" s="13" t="s">
         <v>2</v>
       </c>
@@ -25955,20 +25993,20 @@
       <c r="M1" s="89"/>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="534" t="s">
+      <c r="A2" s="539" t="s">
         <v>885</v>
       </c>
-      <c r="B2" s="534"/>
-      <c r="C2" s="534"/>
-      <c r="D2" s="534"/>
-      <c r="E2" s="534"/>
-      <c r="F2" s="534"/>
-      <c r="G2" s="534"/>
-      <c r="H2" s="534"/>
-      <c r="I2" s="534"/>
-      <c r="J2" s="534"/>
-      <c r="K2" s="534"/>
-      <c r="L2" s="534"/>
+      <c r="B2" s="539"/>
+      <c r="C2" s="539"/>
+      <c r="D2" s="539"/>
+      <c r="E2" s="539"/>
+      <c r="F2" s="539"/>
+      <c r="G2" s="539"/>
+      <c r="H2" s="539"/>
+      <c r="I2" s="539"/>
+      <c r="J2" s="539"/>
+      <c r="K2" s="539"/>
+      <c r="L2" s="539"/>
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A3" s="137" t="s">
@@ -26126,28 +26164,28 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L4"/>
+  <autoFilter ref="A1:L4" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="49" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="80" fitToPage="1" showAutoFilter="1">
       <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="49" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="80" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="80" fitToPage="1" showAutoFilter="1">
       <selection activeCell="D1" sqref="D1"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="49" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="80" fitToHeight="0" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="2">
@@ -26156,7 +26194,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:H5" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -26169,15 +26207,15 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
     <tabColor indexed="15"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O113"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="153" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A5" sqref="A5:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -26198,36 +26236,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="541" t="s">
+      <c r="A1" s="546" t="s">
         <v>316</v>
       </c>
-      <c r="B1" s="541"/>
-      <c r="C1" s="541"/>
-      <c r="D1" s="541"/>
-      <c r="E1" s="541"/>
-      <c r="F1" s="541"/>
-      <c r="G1" s="541"/>
-      <c r="H1" s="541"/>
-      <c r="I1" s="541"/>
-      <c r="J1" s="541"/>
-      <c r="K1" s="541"/>
-      <c r="L1" s="541"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
+      <c r="K1" s="546"/>
+      <c r="L1" s="546"/>
     </row>
     <row r="2" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="542" t="s">
+      <c r="A2" s="547" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="542"/>
-      <c r="C2" s="542"/>
-      <c r="D2" s="542"/>
-      <c r="E2" s="542"/>
-      <c r="F2" s="542"/>
-      <c r="G2" s="542"/>
-      <c r="H2" s="542"/>
-      <c r="I2" s="542"/>
-      <c r="J2" s="542"/>
-      <c r="K2" s="542"/>
-      <c r="L2" s="542"/>
+      <c r="B2" s="547"/>
+      <c r="C2" s="547"/>
+      <c r="D2" s="547"/>
+      <c r="E2" s="547"/>
+      <c r="F2" s="547"/>
+      <c r="G2" s="547"/>
+      <c r="H2" s="547"/>
+      <c r="I2" s="547"/>
+      <c r="J2" s="547"/>
+      <c r="K2" s="547"/>
+      <c r="L2" s="547"/>
     </row>
     <row r="3" spans="1:15" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59"/>
@@ -26268,10 +26306,10 @@
       <c r="H4" s="65" t="s">
         <v>340</v>
       </c>
-      <c r="I4" s="529" t="s">
+      <c r="I4" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="J4" s="529"/>
+      <c r="J4" s="534"/>
       <c r="K4" s="73" t="s">
         <v>2</v>
       </c>
@@ -26289,20 +26327,20 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="540" t="s">
+      <c r="A5" s="545" t="s">
         <v>309</v>
       </c>
-      <c r="B5" s="540"/>
-      <c r="C5" s="540"/>
-      <c r="D5" s="540"/>
-      <c r="E5" s="540"/>
-      <c r="F5" s="540"/>
-      <c r="G5" s="540"/>
-      <c r="H5" s="540"/>
-      <c r="I5" s="540"/>
-      <c r="J5" s="540"/>
-      <c r="K5" s="540"/>
-      <c r="L5" s="540"/>
+      <c r="B5" s="545"/>
+      <c r="C5" s="545"/>
+      <c r="D5" s="545"/>
+      <c r="E5" s="545"/>
+      <c r="F5" s="545"/>
+      <c r="G5" s="545"/>
+      <c r="H5" s="545"/>
+      <c r="I5" s="545"/>
+      <c r="J5" s="545"/>
+      <c r="K5" s="545"/>
+      <c r="L5" s="545"/>
     </row>
     <row r="6" spans="1:15" s="129" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="368"/>
@@ -27834,30 +27872,30 @@
       <c r="L113" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L2">
+  <autoFilter ref="A1:L2" xr:uid="{00000000-0009-0000-0000-000007000000}">
     <filterColumn colId="4" showButton="0"/>
   </autoFilter>
   <customSheetViews>
-    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="75" fitToPage="1" showAutoFilter="1">
-      <selection activeCell="D4" sqref="D4"/>
+    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="75" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <selection activeCell="C25" sqref="C25"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="78" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
+      <pageSetup scale="52" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
     <customSheetView guid="{5B5A346C-618F-49AC-9181-F5E0B5D30CFD}" scale="75" fitToPage="1" printArea="1" showAutoFilter="1">
       <selection activeCell="P7" sqref="P7"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
       <pageSetup scale="52" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId2"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
-    <customSheetView guid="{E02D8BBA-373C-430A-B0C6-EFAFB65B79B1}" scale="75" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
-      <selection activeCell="C25" sqref="C25"/>
+    <customSheetView guid="{7C423F7C-6103-4542-A65F-815D7082BC2E}" scale="75" fitToPage="1" showAutoFilter="1">
+      <selection activeCell="D4" sqref="D4"/>
       <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
-      <pageSetup scale="52" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId3"/>
+      <pageSetup scale="78" fitToHeight="0" orientation="portrait" verticalDpi="1200" r:id="rId3"/>
       <headerFooter alignWithMargins="0"/>
-      <autoFilter ref="B1:L1"/>
+      <autoFilter ref="B1:L1" xr:uid="{00000000-0000-0000-0000-000000000000}"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="4">
@@ -27868,7 +27906,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H7" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>YearBands</formula1>
     </dataValidation>
   </dataValidations>
@@ -27881,7 +27919,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor indexed="15"/>
     <pageSetUpPr fitToPage="1"/>
@@ -27889,7 +27927,7 @@
   <dimension ref="A1:O115"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" zoomScaleSheetLayoutView="153" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -27910,36 +27948,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="541" t="s">
+      <c r="A1" s="546" t="s">
         <v>316</v>
       </c>
-      <c r="B1" s="541"/>
-      <c r="C1" s="541"/>
-      <c r="D1" s="541"/>
-      <c r="E1" s="541"/>
-      <c r="F1" s="541"/>
-      <c r="G1" s="541"/>
-      <c r="H1" s="541"/>
-      <c r="I1" s="541"/>
-      <c r="J1" s="541"/>
-      <c r="K1" s="541"/>
-      <c r="L1" s="541"/>
+      <c r="B1" s="546"/>
+      <c r="C1" s="546"/>
+      <c r="D1" s="546"/>
+      <c r="E1" s="546"/>
+      <c r="F1" s="546"/>
+      <c r="G1" s="546"/>
+      <c r="H1" s="546"/>
+      <c r="I1" s="546"/>
+      <c r="J1" s="546"/>
+      <c r="K1" s="546"/>
+      <c r="L1" s="546"/>
     </row>
     <row r="2" spans="1:15" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="542" t="s">
+      <c r="A2" s="547" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="542"/>
-      <c r="C2" s="542"/>
-      <c r="D2" s="542"/>
-      <c r="E2" s="542"/>
-      <c r="F2" s="542"/>
-      <c r="G2" s="542"/>
-      <c r="H2" s="542"/>
-      <c r="I2" s="542"/>
-      <c r="J2" s="542"/>
-      <c r="K2" s="542"/>
-      <c r="L2" s="542"/>
+      <c r="B2" s="547"/>
+      <c r="C2" s="547"/>
+      <c r="D2" s="547"/>
+      <c r="E2" s="547"/>
+      <c r="F2" s="547"/>
+      <c r="G2" s="547"/>
+      <c r="H2" s="547"/>
+      <c r="I2" s="547"/>
+      <c r="J2" s="547"/>
+      <c r="K2" s="547"/>
+      <c r="L2" s="547"/>
     </row>
     <row r="3" spans="1:15" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="151"/>
@@ -27980,10 +28018,10 @@
       <c r="H4" s="161" t="s">
         <v>340</v>
       </c>
-      <c r="I4" s="529" t="s">
+      <c r="I4" s="534" t="s">
         <v>341</v>
       </c>
-      <c r="J4" s="529"/>
+      <c r="J4" s="534"/>
       <c r="K4" s="73" t="s">
         <v>2</v>
       </c>
@@ -28001,20 +28039,20 @@
       </c>
     </row>
     <row r="5" spans="1:15" s="19" customFormat="1" ht="20.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="540" t="s">
+      <c r="A5" s="545" t="s">
         <v>647</v>
       </c>
-      <c r="B5" s="540"/>
-      <c r="C5" s="540"/>
-      <c r="D5" s="540"/>
-      <c r="E5" s="540"/>
-      <c r="F5" s="540"/>
-      <c r="G5" s="540"/>
-      <c r="H5" s="540"/>
-      <c r="I5" s="540"/>
-      <c r="J5" s="540"/>
-      <c r="K5" s="540"/>
-      <c r="L5" s="540"/>
+      <c r="B5" s="545"/>
+      <c r="C5" s="545"/>
+      <c r="D5" s="545"/>
+      <c r="E5" s="545"/>
+      <c r="F5" s="545"/>
+      <c r="G5" s="545"/>
+      <c r="H5" s="545"/>
+      <c r="I5" s="545"/>
+      <c r="J5" s="545"/>
+      <c r="K5" s="545"/>
+      <c r="L5" s="545"/>
     </row>
     <row r="6" spans="1:15" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="174" t="s">
@@ -29703,7 +29741,7 @@
       <c r="L115" s="129"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L2">
+  <autoFilter ref="A1:L2" xr:uid="{00000000-0009-0000-0000-000008000000}">
     <filterColumn colId="4" showButton="0"/>
   </autoFilter>
   <mergeCells count="4">

</xml_diff>